<commit_message>
Added F407 V1.2.4 files
</commit_message>
<xml_diff>
--- a/OpenFFBoard-main/V1.2.3 F407/Assembly/JLC BOM STM FFBoard.xlsx
+++ b/OpenFFBoard-main/V1.2.3 F407/Assembly/JLC BOM STM FFBoard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\eagle\projects\OpenFFBoard\Assembly\STM 1.2.3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\git\OpenFFBoard-hardware\OpenFFBoard-main\V1.2.3 F407\Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2196751-782C-41E2-A962-1E4D13FD70F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D388280-A9B0-4CFD-B6F5-D1DA241FD121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14970" yWindow="2415" windowWidth="33690" windowHeight="17490" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18810" yWindow="3315" windowWidth="16695" windowHeight="15165" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
   <si>
     <t>Comment</t>
   </si>
@@ -330,6 +330,15 @@
   </si>
   <si>
     <t>C2827654</t>
+  </si>
+  <si>
+    <t>5x2 Pinheader</t>
+  </si>
+  <si>
+    <t>C358694</t>
+  </si>
+  <si>
+    <t>TH</t>
   </si>
 </sst>
 </file>
@@ -749,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK25"/>
+  <dimension ref="A1:AMK26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1112,6 +1121,17 @@
       </c>
       <c r="D25" s="4" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>